<commit_message>
old database course files undo delete, biom510 exam 2
</commit_message>
<xml_diff>
--- a/LaTech/BIOM_510_Bioinstrumentation/HW/1/HW1.xlsx
+++ b/LaTech/BIOM_510_Bioinstrumentation/HW/1/HW1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunzi\Documents\Study\LaTech\BIOM_510_Bioinstrumentation\HW\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD512A6-EE18-4FFD-9237-B4E0D79F5775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957196B4-24F7-4EA5-84B2-6179A0247319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7680" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{C2151E38-9E59-4B2A-8881-C4899E03746F}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{C2151E38-9E59-4B2A-8881-C4899E03746F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2229,13 +2229,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A039E79-0170-4B68-AFCE-BE92183E00A8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>1.3361564395333771</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>12.667059925007866</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10.1</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>162.3169243496925</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>94.049530896258688</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>90.401109170582984</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10000</v>
       </c>

</xml_diff>